<commit_message>
Cambio en el encapsulado de 4 Resistencias para evitar que salten en el soldado.
</commit_message>
<xml_diff>
--- a/02.HARDWARE/V2-ROVER R-1/02.BOM/BATT_DCDC.xlsx
+++ b/02.HARDWARE/V2-ROVER R-1/02.BOM/BATT_DCDC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Javi\TEAMDR~1\JRODRI~1\Repositorios\01.Rover\02.HARDWARE\V2-ROVER R-1\02.BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Team Dropbox\JRODRIGUEZ\Repositorios\01.Rover\02.HARDWARE\V2-ROVER R-1\02.BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC55AB49-9C11-4EE4-9221-64BAA53E1F3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C0B83C-EE59-4C55-811E-C1F2440F4DEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BATT_DCDC" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="135">
   <si>
     <t>Qty</t>
   </si>
@@ -432,9 +432,6 @@
     <t>220pF, 16V, C0G</t>
   </si>
   <si>
-    <t>YES</t>
-  </si>
-  <si>
     <t>J1</t>
   </si>
   <si>
@@ -451,6 +448,9 @@
   </si>
   <si>
     <t>Se añade la posicion 38.</t>
+  </si>
+  <si>
+    <t>Las posiciones 21,27,28 y 35 cambian su Package a SMD 0603</t>
   </si>
 </sst>
 </file>
@@ -683,7 +683,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="39">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -890,12 +890,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1135,7 +1129,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1183,9 +1177,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1198,6 +1189,10 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1244,82 +1239,7 @@
     <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="13">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1372,6 +1292,31 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}"/>
@@ -1388,14 +1333,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AD639D9D-BFED-4687-9866-69587ACF8311}" name="Tabla1" displayName="Tabla1" ref="A6:J44" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AD639D9D-BFED-4687-9866-69587ACF8311}" name="Tabla1" displayName="Tabla1" ref="A6:J44" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2" tableBorderDxfId="1">
   <autoFilter ref="A6:J44" xr:uid="{AD639D9D-BFED-4687-9866-69587ACF8311}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:J38">
     <sortCondition ref="D6:D38"/>
   </sortState>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{A4EEF5D5-EC32-4E92-A16D-A2C00D09EC58}" name="Position"/>
-    <tableColumn id="10" xr3:uid="{AB092131-4167-465E-A2DF-04757A83F427}" name="NEW" dataDxfId="9"/>
+    <tableColumn id="10" xr3:uid="{AB092131-4167-465E-A2DF-04757A83F427}" name="NEW" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{958FBBFD-8FA4-4642-8441-E180A56F96F0}" name="Qty"/>
     <tableColumn id="3" xr3:uid="{FBAE2CFA-77A4-45AD-9266-0EFC588D4B64}" name="Part"/>
     <tableColumn id="4" xr3:uid="{FB9BFB6E-6495-468E-802B-025835AD898D}" name="Value"/>
@@ -1698,7 +1643,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1708,8 +1653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45:XFD45"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1732,7 +1677,7 @@
       </c>
       <c r="B2" s="3">
         <f>MAX(_HISTORY!A4:A55)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="27" x14ac:dyDescent="0.4">
@@ -1742,12 +1687,12 @@
       <c r="D3" s="4"/>
     </row>
     <row r="4" spans="1:10" ht="27" x14ac:dyDescent="0.4">
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="24"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="23"/>
     </row>
     <row r="5" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="6"/>
@@ -2296,8 +2241,8 @@
       <c r="F27" t="s">
         <v>63</v>
       </c>
-      <c r="G27" t="s">
-        <v>64</v>
+      <c r="G27" s="26" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -2434,8 +2379,8 @@
       <c r="F33" t="s">
         <v>63</v>
       </c>
-      <c r="G33" t="s">
-        <v>64</v>
+      <c r="G33" s="26" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -2457,8 +2402,8 @@
       <c r="F34" t="s">
         <v>63</v>
       </c>
-      <c r="G34" t="s">
-        <v>64</v>
+      <c r="G34" s="26" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -2488,8 +2433,8 @@
       <c r="A36">
         <v>30</v>
       </c>
-      <c r="B36" s="21" t="s">
-        <v>128</v>
+      <c r="B36" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -2627,8 +2572,8 @@
       <c r="F41" t="s">
         <v>63</v>
       </c>
-      <c r="G41" t="s">
-        <v>64</v>
+      <c r="G41" s="26" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
@@ -2682,25 +2627,25 @@
         <v>38</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>128</v>
+        <v>75</v>
       </c>
       <c r="C44">
         <v>1</v>
       </c>
       <c r="D44" t="s">
+        <v>128</v>
+      </c>
+      <c r="E44" t="s">
         <v>129</v>
       </c>
-      <c r="E44" t="s">
+      <c r="F44" t="s">
         <v>130</v>
       </c>
-      <c r="F44" t="s">
+      <c r="G44" t="s">
         <v>131</v>
       </c>
-      <c r="G44" t="s">
+      <c r="J44" s="20" t="s">
         <v>132</v>
-      </c>
-      <c r="J44" s="20" t="s">
-        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -2708,13 +2653,13 @@
     <mergeCell ref="B4:E4"/>
   </mergeCells>
   <conditionalFormatting sqref="B7:B44">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",B7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="YES">
+    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="YES">
       <formula>NOT(ISERROR(SEARCH("YES",B7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",B7)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2738,15 +2683,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5396D425-0A04-B64D-B9F7-D3F9797B3C5D}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="51.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.140625" style="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
@@ -2764,7 +2709,7 @@
       <c r="C3" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="25" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2778,7 +2723,7 @@
       <c r="C4" t="s">
         <v>90</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="19" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2810,7 +2755,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
@@ -2820,7 +2765,7 @@
       <c r="C7" t="s">
         <v>92</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="19" t="s">
         <v>115</v>
       </c>
     </row>
@@ -2834,7 +2779,21 @@
       <c r="C8" t="s">
         <v>90</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="19" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" s="17">
+        <v>45062</v>
+      </c>
+      <c r="C9" t="s">
+        <v>90</v>
+      </c>
+      <c r="D9" s="19" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2854,11 +2813,11 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
     </row>
     <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">

</xml_diff>

<commit_message>
Inclusión de un sustitutivo del transistor de salida del DCDC
#66
</commit_message>
<xml_diff>
--- a/02.HARDWARE/V2-ROVER R-1/02.BOM/BATT_DCDC.xlsx
+++ b/02.HARDWARE/V2-ROVER R-1/02.BOM/BATT_DCDC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Team Dropbox\JRODRIGUEZ\Repositorios\01.Rover\02.HARDWARE\V2-ROVER R-1\02.BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C0B83C-EE59-4C55-811E-C1F2440F4DEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A74C31-7BBD-484A-9AF6-E7A840A9E0EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BATT_DCDC" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="137">
   <si>
     <t>Qty</t>
   </si>
@@ -451,6 +451,12 @@
   </si>
   <si>
     <t>Las posiciones 21,27,28 y 35 cambian su Package a SMD 0603</t>
+  </si>
+  <si>
+    <t>Sustituto</t>
+  </si>
+  <si>
+    <t>RQ3G110ATTB</t>
   </si>
 </sst>
 </file>
@@ -1129,7 +1135,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1177,6 +1183,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="29" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1189,10 +1198,6 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1240,6 +1245,31 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="7">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1292,31 +1322,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}"/>
@@ -1333,14 +1338,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AD639D9D-BFED-4687-9866-69587ACF8311}" name="Tabla1" displayName="Tabla1" ref="A6:J44" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2" tableBorderDxfId="1">
-  <autoFilter ref="A6:J44" xr:uid="{AD639D9D-BFED-4687-9866-69587ACF8311}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AD639D9D-BFED-4687-9866-69587ACF8311}" name="Tabla1" displayName="Tabla1" ref="A6:K44" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4">
+  <autoFilter ref="A6:K44" xr:uid="{AD639D9D-BFED-4687-9866-69587ACF8311}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:J38">
     <sortCondition ref="D6:D38"/>
   </sortState>
-  <tableColumns count="10">
+  <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{A4EEF5D5-EC32-4E92-A16D-A2C00D09EC58}" name="Position"/>
-    <tableColumn id="10" xr3:uid="{AB092131-4167-465E-A2DF-04757A83F427}" name="NEW" dataDxfId="0"/>
+    <tableColumn id="10" xr3:uid="{AB092131-4167-465E-A2DF-04757A83F427}" name="NEW" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{958FBBFD-8FA4-4642-8441-E180A56F96F0}" name="Qty"/>
     <tableColumn id="3" xr3:uid="{FBAE2CFA-77A4-45AD-9266-0EFC588D4B64}" name="Part"/>
     <tableColumn id="4" xr3:uid="{FB9BFB6E-6495-468E-802B-025835AD898D}" name="Value"/>
@@ -1348,7 +1353,8 @@
     <tableColumn id="6" xr3:uid="{054D275A-2D21-4AFA-9C9D-0B7B74A00644}" name="Package"/>
     <tableColumn id="7" xr3:uid="{D4D5910B-60E5-4F90-9C90-C3505AD00BB9}" name="Unit Price"/>
     <tableColumn id="8" xr3:uid="{69DE7A27-EA56-4539-9436-4BE17DA44A72}" name="Extended Price"/>
-    <tableColumn id="9" xr3:uid="{A2D6CBAE-280A-4BCB-929A-9135FF379154}" name="Link"/>
+    <tableColumn id="9" xr3:uid="{A2D6CBAE-280A-4BCB-929A-9135FF379154}" name="Sustituto"/>
+    <tableColumn id="11" xr3:uid="{9A134734-C129-4A70-B805-F1DAA6862DF9}" name="Link"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1651,10 +1657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J44"/>
+  <dimension ref="A1:K44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1666,12 +1672,14 @@
     <col min="6" max="7" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="145.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>56</v>
       </c>
@@ -1680,27 +1688,27 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="27" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11" ht="27" x14ac:dyDescent="0.4">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
       <c r="D3" s="4"/>
     </row>
-    <row r="4" spans="1:10" ht="27" x14ac:dyDescent="0.4">
-      <c r="B4" s="21" t="s">
+    <row r="4" spans="1:11" ht="27" x14ac:dyDescent="0.4">
+      <c r="B4" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="23"/>
-    </row>
-    <row r="5" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="24"/>
+    </row>
+    <row r="5" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="6"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="8"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>58</v>
       </c>
@@ -1729,10 +1737,13 @@
         <v>61</v>
       </c>
       <c r="J6" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="K6" s="9" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1755,7 +1766,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -1778,7 +1789,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
@@ -1801,7 +1812,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>4</v>
       </c>
@@ -1824,7 +1835,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>5</v>
       </c>
@@ -1847,7 +1858,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="18">
         <v>6</v>
       </c>
@@ -1875,11 +1886,12 @@
       <c r="I12" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="J12" s="18" t="s">
+      <c r="J12" s="18"/>
+      <c r="K12" s="18" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>7</v>
       </c>
@@ -1902,7 +1914,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="18">
         <v>8</v>
       </c>
@@ -1930,11 +1942,12 @@
       <c r="I14" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="J14" s="18" t="s">
+      <c r="J14" s="18"/>
+      <c r="K14" s="18" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>9</v>
       </c>
@@ -1957,7 +1970,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>10</v>
       </c>
@@ -1979,11 +1992,12 @@
       <c r="G16" t="s">
         <v>15</v>
       </c>
-      <c r="J16" s="20" t="s">
+      <c r="J16" s="20"/>
+      <c r="K16" s="20" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>11</v>
       </c>
@@ -2005,11 +2019,12 @@
       <c r="G17" t="s">
         <v>116</v>
       </c>
-      <c r="J17" s="20" t="s">
+      <c r="J17" s="20"/>
+      <c r="K17" s="20" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>12</v>
       </c>
@@ -2031,11 +2046,12 @@
       <c r="G18" t="s">
         <v>119</v>
       </c>
-      <c r="J18" s="20" t="s">
+      <c r="J18" s="20"/>
+      <c r="K18" s="20" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>13</v>
       </c>
@@ -2058,10 +2074,13 @@
         <v>94</v>
       </c>
       <c r="J19" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="K19" s="20" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>14</v>
       </c>
@@ -2084,7 +2103,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>15</v>
       </c>
@@ -2107,7 +2126,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>16</v>
       </c>
@@ -2130,7 +2149,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>17</v>
       </c>
@@ -2153,7 +2172,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>18</v>
       </c>
@@ -2176,7 +2195,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>19</v>
       </c>
@@ -2199,7 +2218,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>20</v>
       </c>
@@ -2222,7 +2241,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>21</v>
       </c>
@@ -2241,11 +2260,11 @@
       <c r="F27" t="s">
         <v>63</v>
       </c>
-      <c r="G27" s="26" t="s">
+      <c r="G27" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>22</v>
       </c>
@@ -2268,7 +2287,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>23</v>
       </c>
@@ -2291,7 +2310,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>24</v>
       </c>
@@ -2314,7 +2333,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>25</v>
       </c>
@@ -2337,7 +2356,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>26</v>
       </c>
@@ -2360,7 +2379,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>27</v>
       </c>
@@ -2379,11 +2398,11 @@
       <c r="F33" t="s">
         <v>63</v>
       </c>
-      <c r="G33" s="26" t="s">
+      <c r="G33" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>28</v>
       </c>
@@ -2402,11 +2421,11 @@
       <c r="F34" t="s">
         <v>63</v>
       </c>
-      <c r="G34" s="26" t="s">
+      <c r="G34" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>29</v>
       </c>
@@ -2429,7 +2448,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>30</v>
       </c>
@@ -2451,11 +2470,12 @@
       <c r="G36" t="s">
         <v>121</v>
       </c>
-      <c r="J36" s="20" t="s">
+      <c r="J36" s="20"/>
+      <c r="K36" s="20" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>31</v>
       </c>
@@ -2477,11 +2497,12 @@
       <c r="G37" t="s">
         <v>73</v>
       </c>
-      <c r="J37" s="20" t="s">
+      <c r="J37" s="20"/>
+      <c r="K37" s="20" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>32</v>
       </c>
@@ -2503,11 +2524,12 @@
       <c r="G38" t="s">
         <v>126</v>
       </c>
-      <c r="J38" s="20" t="s">
+      <c r="J38" s="20"/>
+      <c r="K38" s="20" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>33</v>
       </c>
@@ -2530,7 +2552,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>34</v>
       </c>
@@ -2553,7 +2575,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>35</v>
       </c>
@@ -2572,11 +2594,11 @@
       <c r="F41" t="s">
         <v>63</v>
       </c>
-      <c r="G41" s="26" t="s">
+      <c r="G41" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>36</v>
       </c>
@@ -2599,7 +2621,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>37</v>
       </c>
@@ -2622,7 +2644,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>38</v>
       </c>
@@ -2644,7 +2666,8 @@
       <c r="G44" t="s">
         <v>131</v>
       </c>
-      <c r="J44" s="20" t="s">
+      <c r="J44" s="20"/>
+      <c r="K44" s="20" t="s">
         <v>132</v>
       </c>
     </row>
@@ -2653,30 +2676,31 @@
     <mergeCell ref="B4:E4"/>
   </mergeCells>
   <conditionalFormatting sqref="B7:B44">
-    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",B7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="YES">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="YES">
       <formula>NOT(ISERROR(SEARCH("YES",B7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",B7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="J16" r:id="rId1" xr:uid="{4EF74C74-5599-D341-A184-4262A41DCCB8}"/>
-    <hyperlink ref="J17" r:id="rId2" xr:uid="{25F4A353-B9E3-8846-9826-52724C670B5F}"/>
-    <hyperlink ref="J18" r:id="rId3" xr:uid="{B4F6A03A-A5DE-9B42-92BD-39D8294FBCE8}"/>
-    <hyperlink ref="J19" r:id="rId4" xr:uid="{9CE05E9A-D9C3-4A45-8F2A-3443DA782029}"/>
-    <hyperlink ref="J36" r:id="rId5" xr:uid="{C813FBCD-BBA9-7C41-B5BA-B64FA046AB8A}"/>
-    <hyperlink ref="J37" r:id="rId6" xr:uid="{0374EAFF-2FDA-AA4E-A136-EB33DA6E9CFA}"/>
-    <hyperlink ref="J38" r:id="rId7" xr:uid="{11C11D1A-BC77-584C-84B8-7A63B99051B2}"/>
-    <hyperlink ref="J44" r:id="rId8" xr:uid="{5EDC74FA-60E2-4774-B3DE-D870CDFE642B}"/>
+    <hyperlink ref="K16" r:id="rId1" xr:uid="{4EF74C74-5599-D341-A184-4262A41DCCB8}"/>
+    <hyperlink ref="K17" r:id="rId2" xr:uid="{25F4A353-B9E3-8846-9826-52724C670B5F}"/>
+    <hyperlink ref="K18" r:id="rId3" xr:uid="{B4F6A03A-A5DE-9B42-92BD-39D8294FBCE8}"/>
+    <hyperlink ref="K19" r:id="rId4" xr:uid="{9CE05E9A-D9C3-4A45-8F2A-3443DA782029}"/>
+    <hyperlink ref="K36" r:id="rId5" xr:uid="{C813FBCD-BBA9-7C41-B5BA-B64FA046AB8A}"/>
+    <hyperlink ref="K37" r:id="rId6" xr:uid="{0374EAFF-2FDA-AA4E-A136-EB33DA6E9CFA}"/>
+    <hyperlink ref="K38" r:id="rId7" xr:uid="{11C11D1A-BC77-584C-84B8-7A63B99051B2}"/>
+    <hyperlink ref="K44" r:id="rId8" xr:uid="{5EDC74FA-60E2-4774-B3DE-D870CDFE642B}"/>
+    <hyperlink ref="J19" r:id="rId9" xr:uid="{A0D7275C-8A9F-4246-B171-83ADE8AF708D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
   <tableParts count="1">
-    <tablePart r:id="rId10"/>
+    <tablePart r:id="rId11"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2686,7 +2710,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2709,7 +2733,7 @@
       <c r="C3" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="21" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2813,11 +2837,11 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
     </row>
     <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">

</xml_diff>

<commit_message>
Revision antes de enviar a SETI 3ra produccion
Se actuliza la columna NEW
</commit_message>
<xml_diff>
--- a/02.HARDWARE/V2-ROVER R-1/02.BOM/BATT_DCDC.xlsx
+++ b/02.HARDWARE/V2-ROVER R-1/02.BOM/BATT_DCDC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Team Dropbox\JRODRIGUEZ\Repositorios\01.Rover\02.HARDWARE\V2-ROVER R-1\02.BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reozen/Team Dropbox/David Garrido/MUSOTOKU/PROJECTS/BATTERYPACK - FALCON/00.REPOSITORIES/BATTERY-PACK/02.HARDWARE/V2-ROVER R-1/02.BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32FE5ED3-2977-41E5-B16B-8327EF248036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33A685F2-B57E-364A-862C-0D5E68094134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20" yWindow="500" windowWidth="34400" windowHeight="26580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BATT_DCDC" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="148">
   <si>
     <t>Qty</t>
   </si>
@@ -487,12 +487,18 @@
   <si>
     <t>Se elimina el part Q5 de la posicion 14</t>
   </si>
+  <si>
+    <t xml:space="preserve">MAX5048 </t>
+  </si>
+  <si>
+    <t>Se actuliza la columna NEW</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="30" x14ac:knownFonts="1">
+  <fonts count="31">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -716,6 +722,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="ArialMT"/>
     </font>
   </fonts>
   <fills count="38">
@@ -1164,7 +1175,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1228,51 +1239,52 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
-    <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Bueno" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Encabezado 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Encabezado 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Énfasis1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Énfasis2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Énfasis3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Énfasis4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Énfasis5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Énfasis6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Hipervínculo" xfId="42" builtinId="8"/>
-    <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Salida" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Texto de advertencia" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Texto explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="7">
     <dxf>
@@ -1369,9 +1381,8 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AD639D9D-BFED-4687-9866-69587ACF8311}" name="Tabla1" displayName="Tabla1" ref="A6:K46" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4">
-  <autoFilter ref="A6:K46" xr:uid="{AD639D9D-BFED-4687-9866-69587ACF8311}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:K46">
-    <sortCondition ref="D6:D46"/>
+    <sortCondition ref="A6:A46"/>
   </sortState>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{A4EEF5D5-EC32-4E92-A16D-A2C00D09EC58}" name="Position"/>
@@ -1391,7 +1402,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1689,42 +1700,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="145.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="145.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="16">
       <c r="A2" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B2" s="3">
         <f>MAX(_HISTORY!A4:A55)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="27" x14ac:dyDescent="0.4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="26">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
       <c r="D3" s="4"/>
     </row>
-    <row r="4" spans="1:11" ht="27" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:11" ht="26">
       <c r="B4" s="23" t="s">
         <v>55</v>
       </c>
@@ -1732,13 +1743,13 @@
       <c r="D4" s="24"/>
       <c r="E4" s="25"/>
     </row>
-    <row r="5" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:11" ht="13.5" customHeight="1">
       <c r="B5" s="6"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="8"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6" s="9" t="s">
         <v>56</v>
       </c>
@@ -1773,7 +1784,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1796,7 +1807,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="A8">
         <v>2</v>
       </c>
@@ -1819,7 +1830,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11">
       <c r="A9">
         <v>3</v>
       </c>
@@ -1842,7 +1853,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11">
       <c r="A10">
         <v>4</v>
       </c>
@@ -1865,7 +1876,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11">
       <c r="A11">
         <v>5</v>
       </c>
@@ -1888,78 +1899,98 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="12" spans="1:11">
+      <c r="A12" s="18">
+        <v>6</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="G12" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="H12" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="I12" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13">
         <v>7</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="B13" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
         <v>12</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E13" t="s">
         <v>110</v>
-      </c>
-      <c r="F12" t="s">
-        <v>69</v>
-      </c>
-      <c r="G12" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>9</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" t="s">
-        <v>111</v>
       </c>
       <c r="F13" t="s">
         <v>69</v>
       </c>
       <c r="G13" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>33</v>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="18">
+        <v>8</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14" t="s">
-        <v>95</v>
-      </c>
-      <c r="E14" t="s">
-        <v>125</v>
-      </c>
-      <c r="F14" t="s">
-        <v>69</v>
-      </c>
-      <c r="G14" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C14" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="G14" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="H14" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="I14" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>73</v>
@@ -1968,19 +1999,19 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>96</v>
+        <v>6</v>
       </c>
       <c r="E15" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
       <c r="F15" t="s">
         <v>69</v>
       </c>
       <c r="G15" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16">
         <v>10</v>
       </c>
@@ -2007,7 +2038,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="A17">
         <v>11</v>
       </c>
@@ -2034,129 +2065,111 @@
         <v>115</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="18">
-        <v>6</v>
+    <row r="18" spans="1:11">
+      <c r="A18">
+        <v>12</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C18" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="D18" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="E18" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="F18" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="G18" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="H18" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="I18" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="J18" s="18"/>
-      <c r="K18" s="18" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="18">
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" t="s">
+        <v>65</v>
+      </c>
+      <c r="G18" t="s">
+        <v>117</v>
+      </c>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19">
+        <v>13</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>51</v>
+      </c>
+      <c r="E19" t="s">
+        <v>50</v>
+      </c>
+      <c r="F19" t="s">
+        <v>67</v>
+      </c>
+      <c r="G19" t="s">
+        <v>92</v>
+      </c>
+      <c r="J19" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="K19" s="20" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20">
+        <v>14</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>144</v>
+      </c>
+      <c r="E20" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" t="s">
+        <v>67</v>
+      </c>
+      <c r="G20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21">
+        <v>15</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C19" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="D19" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="E19" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="F19" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="G19" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="H19" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="I19" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="J19" s="18"/>
-      <c r="K19" s="18" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>38</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20" t="s">
-        <v>126</v>
-      </c>
-      <c r="E20" t="s">
-        <v>127</v>
-      </c>
-      <c r="F20" t="s">
-        <v>128</v>
-      </c>
-      <c r="G20" t="s">
-        <v>129</v>
-      </c>
-      <c r="J20" s="20"/>
-      <c r="K20" s="20" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>12</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-      <c r="D21" t="s">
-        <v>11</v>
-      </c>
       <c r="E21" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F21" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G21" t="s">
-        <v>117</v>
-      </c>
-      <c r="J21" s="20"/>
-      <c r="K21" s="20" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
       <c r="A22">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>73</v>
@@ -2165,27 +2178,21 @@
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="E22" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="F22" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="G22" t="s">
-        <v>92</v>
-      </c>
-      <c r="J22" s="20" t="s">
-        <v>134</v>
-      </c>
-      <c r="K22" s="20" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
       <c r="A23">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>73</v>
@@ -2194,21 +2201,21 @@
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>144</v>
+        <v>33</v>
       </c>
       <c r="E23" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="F23" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="G23" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
       <c r="A24">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>73</v>
@@ -2217,10 +2224,10 @@
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="E24" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="F24" t="s">
         <v>61</v>
@@ -2229,9 +2236,9 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="A25">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>73</v>
@@ -2240,10 +2247,10 @@
         <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="E25" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="F25" t="s">
         <v>61</v>
@@ -2252,9 +2259,9 @@
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11">
       <c r="A26">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>73</v>
@@ -2263,10 +2270,10 @@
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="E26" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="F26" t="s">
         <v>61</v>
@@ -2275,9 +2282,9 @@
         <v>62</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11">
       <c r="A27">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>73</v>
@@ -2286,33 +2293,33 @@
         <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>43</v>
+        <v>101</v>
       </c>
       <c r="E27" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="F27" t="s">
         <v>61</v>
       </c>
       <c r="G27" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
       <c r="A28">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D28" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E28" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F28" t="s">
         <v>61</v>
@@ -2321,21 +2328,21 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11">
       <c r="A29">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>73</v>
+        <v>135</v>
       </c>
       <c r="C29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>102</v>
+        <v>143</v>
       </c>
       <c r="E29" t="s">
-        <v>103</v>
+        <v>4</v>
       </c>
       <c r="F29" t="s">
         <v>61</v>
@@ -2344,21 +2351,21 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11">
       <c r="A30">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>135</v>
+        <v>73</v>
       </c>
       <c r="C30">
         <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>140</v>
+        <v>31</v>
       </c>
       <c r="E30" t="s">
-        <v>141</v>
+        <v>106</v>
       </c>
       <c r="F30" t="s">
         <v>61</v>
@@ -2367,9 +2374,9 @@
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11">
       <c r="A31">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>73</v>
@@ -2378,10 +2385,10 @@
         <v>1</v>
       </c>
       <c r="D31" t="s">
-        <v>104</v>
+        <v>17</v>
       </c>
       <c r="E31" t="s">
-        <v>105</v>
+        <v>16</v>
       </c>
       <c r="F31" t="s">
         <v>61</v>
@@ -2390,21 +2397,21 @@
         <v>62</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11">
       <c r="A32">
+        <v>26</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32" t="s">
+        <v>21</v>
+      </c>
+      <c r="E32" t="s">
         <v>20</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C32">
-        <v>1</v>
-      </c>
-      <c r="D32" t="s">
-        <v>25</v>
-      </c>
-      <c r="E32" t="s">
-        <v>24</v>
       </c>
       <c r="F32" t="s">
         <v>61</v>
@@ -2413,9 +2420,9 @@
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11">
       <c r="A33">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>73</v>
@@ -2424,10 +2431,10 @@
         <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>101</v>
+        <v>37</v>
       </c>
       <c r="E33" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="F33" t="s">
         <v>61</v>
@@ -2436,32 +2443,32 @@
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11">
       <c r="A34">
+        <v>28</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34" t="s">
+        <v>23</v>
+      </c>
+      <c r="E34" t="s">
         <v>22</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C34">
-        <v>2</v>
-      </c>
-      <c r="D34" t="s">
-        <v>39</v>
-      </c>
-      <c r="E34" t="s">
-        <v>38</v>
       </c>
       <c r="F34" t="s">
         <v>61</v>
       </c>
       <c r="G34" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
       <c r="A35">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>73</v>
@@ -2470,10 +2477,10 @@
         <v>1</v>
       </c>
       <c r="D35" t="s">
-        <v>143</v>
+        <v>35</v>
       </c>
       <c r="E35" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="F35" t="s">
         <v>61</v>
@@ -2482,9 +2489,9 @@
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11">
       <c r="A36">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>73</v>
@@ -2493,44 +2500,52 @@
         <v>1</v>
       </c>
       <c r="D36" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="E36" t="s">
-        <v>106</v>
+        <v>121</v>
       </c>
       <c r="F36" t="s">
         <v>61</v>
       </c>
       <c r="G36" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+      <c r="J36" s="20"/>
+      <c r="K36" s="20" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
       <c r="A37">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C37">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D37" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="E37" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="F37" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="G37" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="J37" s="20"/>
+      <c r="K37" s="20" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
       <c r="A38">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>73</v>
@@ -2539,21 +2554,25 @@
         <v>1</v>
       </c>
       <c r="D38" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="E38" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="F38" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="G38" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+      <c r="J38" s="20"/>
+      <c r="K38" s="20" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
       <c r="A39">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>73</v>
@@ -2562,21 +2581,21 @@
         <v>1</v>
       </c>
       <c r="D39" t="s">
-        <v>37</v>
+        <v>95</v>
       </c>
       <c r="E39" t="s">
-        <v>36</v>
+        <v>125</v>
       </c>
       <c r="F39" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="G39" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11">
       <c r="A40">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>73</v>
@@ -2585,21 +2604,21 @@
         <v>1</v>
       </c>
       <c r="D40" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E40" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F40" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="G40" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11">
       <c r="A41">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>73</v>
@@ -2608,10 +2627,10 @@
         <v>1</v>
       </c>
       <c r="D41" t="s">
-        <v>23</v>
+        <v>99</v>
       </c>
       <c r="E41" t="s">
-        <v>22</v>
+        <v>100</v>
       </c>
       <c r="F41" t="s">
         <v>61</v>
@@ -2620,21 +2639,21 @@
         <v>63</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11">
       <c r="A42">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C42">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D42" t="s">
-        <v>35</v>
+        <v>102</v>
       </c>
       <c r="E42" t="s">
-        <v>34</v>
+        <v>103</v>
       </c>
       <c r="F42" t="s">
         <v>61</v>
@@ -2643,9 +2662,9 @@
         <v>62</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11">
       <c r="A43">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>73</v>
@@ -2654,50 +2673,46 @@
         <v>1</v>
       </c>
       <c r="D43" t="s">
-        <v>5</v>
+        <v>104</v>
       </c>
       <c r="E43" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="F43" t="s">
         <v>61</v>
       </c>
       <c r="G43" t="s">
-        <v>119</v>
-      </c>
-      <c r="J43" s="20"/>
-      <c r="K43" s="20" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
       <c r="A44">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C44">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D44" t="s">
-        <v>49</v>
+        <v>126</v>
       </c>
       <c r="E44" t="s">
-        <v>48</v>
+        <v>127</v>
       </c>
       <c r="F44" t="s">
-        <v>68</v>
+        <v>128</v>
       </c>
       <c r="G44" t="s">
-        <v>71</v>
+        <v>129</v>
       </c>
       <c r="J44" s="20"/>
       <c r="K44" s="20" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
       <c r="A45">
         <v>39</v>
       </c>
@@ -2719,35 +2734,34 @@
       <c r="G45" t="s">
         <v>138</v>
       </c>
+      <c r="J45" s="27" t="s">
+        <v>146</v>
+      </c>
       <c r="K45" s="20" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11">
       <c r="A46">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>73</v>
+        <v>135</v>
       </c>
       <c r="C46">
         <v>1</v>
       </c>
       <c r="D46" t="s">
-        <v>53</v>
+        <v>140</v>
       </c>
       <c r="E46" t="s">
-        <v>52</v>
+        <v>141</v>
       </c>
       <c r="F46" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="G46" t="s">
-        <v>124</v>
-      </c>
-      <c r="J46" s="20"/>
-      <c r="K46" s="20" t="s">
-        <v>123</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -2768,13 +2782,13 @@
   <hyperlinks>
     <hyperlink ref="K16" r:id="rId1" xr:uid="{4EF74C74-5599-D341-A184-4262A41DCCB8}"/>
     <hyperlink ref="K17" r:id="rId2" xr:uid="{25F4A353-B9E3-8846-9826-52724C670B5F}"/>
-    <hyperlink ref="K21" r:id="rId3" xr:uid="{B4F6A03A-A5DE-9B42-92BD-39D8294FBCE8}"/>
-    <hyperlink ref="K22" r:id="rId4" xr:uid="{9CE05E9A-D9C3-4A45-8F2A-3443DA782029}"/>
-    <hyperlink ref="K43" r:id="rId5" xr:uid="{C813FBCD-BBA9-7C41-B5BA-B64FA046AB8A}"/>
-    <hyperlink ref="K44" r:id="rId6" xr:uid="{0374EAFF-2FDA-AA4E-A136-EB33DA6E9CFA}"/>
-    <hyperlink ref="K46" r:id="rId7" xr:uid="{11C11D1A-BC77-584C-84B8-7A63B99051B2}"/>
-    <hyperlink ref="K20" r:id="rId8" xr:uid="{5EDC74FA-60E2-4774-B3DE-D870CDFE642B}"/>
-    <hyperlink ref="J22" r:id="rId9" xr:uid="{A0D7275C-8A9F-4246-B171-83ADE8AF708D}"/>
+    <hyperlink ref="K18" r:id="rId3" xr:uid="{B4F6A03A-A5DE-9B42-92BD-39D8294FBCE8}"/>
+    <hyperlink ref="K19" r:id="rId4" xr:uid="{9CE05E9A-D9C3-4A45-8F2A-3443DA782029}"/>
+    <hyperlink ref="K36" r:id="rId5" xr:uid="{C813FBCD-BBA9-7C41-B5BA-B64FA046AB8A}"/>
+    <hyperlink ref="K37" r:id="rId6" xr:uid="{0374EAFF-2FDA-AA4E-A136-EB33DA6E9CFA}"/>
+    <hyperlink ref="K38" r:id="rId7" xr:uid="{11C11D1A-BC77-584C-84B8-7A63B99051B2}"/>
+    <hyperlink ref="K44" r:id="rId8" xr:uid="{5EDC74FA-60E2-4774-B3DE-D870CDFE642B}"/>
+    <hyperlink ref="J19" r:id="rId9" xr:uid="{A0D7275C-8A9F-4246-B171-83ADE8AF708D}"/>
     <hyperlink ref="K45" r:id="rId10" xr:uid="{1506D992-264B-48A9-BCB6-2261D61EAEEF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2787,23 +2801,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5396D425-0A04-B64D-B9F7-D3F9797B3C5D}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="51.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.1640625" style="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="24">
       <c r="A1" s="15" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="20">
       <c r="A3" s="16" t="s">
         <v>84</v>
       </c>
@@ -2817,7 +2831,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="16">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2831,7 +2845,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="64">
       <c r="A5">
         <v>2</v>
       </c>
@@ -2845,7 +2859,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="144">
       <c r="A6">
         <v>3</v>
       </c>
@@ -2859,7 +2873,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="32">
       <c r="A7">
         <v>4</v>
       </c>
@@ -2873,7 +2887,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="16">
       <c r="A8">
         <v>5</v>
       </c>
@@ -2887,7 +2901,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="16">
       <c r="A9">
         <v>6</v>
       </c>
@@ -2901,7 +2915,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="64">
       <c r="A10">
         <v>7</v>
       </c>
@@ -2915,7 +2929,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="16">
       <c r="A11">
         <v>8</v>
       </c>
@@ -2927,6 +2941,20 @@
       </c>
       <c r="D11" s="19" t="s">
         <v>145</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="16">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12" s="22">
+        <v>45195</v>
+      </c>
+      <c r="C12" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -2942,56 +2970,56 @@
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="21">
       <c r="A1" s="26" t="s">
         <v>74</v>
       </c>
       <c r="B1" s="26"/>
       <c r="C1" s="26"/>
     </row>
-    <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="19">
       <c r="A2" s="10" t="s">
         <v>75</v>
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="11"/>
     </row>
-    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="19">
       <c r="A3" s="10" t="s">
         <v>76</v>
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="11"/>
     </row>
-    <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="19">
       <c r="A4" s="10">
         <v>28805</v>
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
     </row>
-    <row r="5" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="19">
       <c r="A5" s="10" t="s">
         <v>77</v>
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="11"/>
     </row>
-    <row r="6" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="19">
       <c r="A6" s="10" t="s">
         <v>78</v>
       </c>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
     </row>
-    <row r="7" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="19">
       <c r="A7" s="10"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
     </row>
-    <row r="8" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="19">
       <c r="A8" s="12" t="s">
         <v>79</v>
       </c>
@@ -3000,7 +3028,7 @@
       </c>
       <c r="C8" s="14"/>
     </row>
-    <row r="9" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="19">
       <c r="A9" s="12" t="s">
         <v>81</v>
       </c>

</xml_diff>

<commit_message>
Actualizacion de la BOM
Esquema de resistencia de balastro,
</commit_message>
<xml_diff>
--- a/02.HARDWARE/V2-ROVER R-1/02.BOM/BATT_DCDC.xlsx
+++ b/02.HARDWARE/V2-ROVER R-1/02.BOM/BATT_DCDC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reozen/Team Dropbox/David Garrido/MUSOTOKU/PROJECTS/BATTERYPACK - FALCON/00.REPOSITORIES/BATTERY-PACK/02.HARDWARE/V2-ROVER R-1/02.BOM/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Team Dropbox\JRODRIGUEZ\Repositorios\01.Rover\02.HARDWARE\V2-ROVER R-1\02.BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33A685F2-B57E-364A-862C-0D5E68094134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86053A1B-EE14-4C5F-BBC9-488F0E9221A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="500" windowWidth="34400" windowHeight="26580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BATT_DCDC" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="155">
   <si>
     <t>Qty</t>
   </si>
@@ -98,9 +98,6 @@
   </si>
   <si>
     <t>33R</t>
-  </si>
-  <si>
-    <t>R5</t>
   </si>
   <si>
     <t>36k</t>
@@ -492,6 +489,32 @@
   </si>
   <si>
     <t>Se actuliza la columna NEW</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>PMV20XNER</t>
+  </si>
+  <si>
+    <t>PMV20XNERSOT23-TO-236AB_NEX-L</t>
+  </si>
+  <si>
+    <t>SOT23-TO-236AB_NEX-L</t>
+  </si>
+  <si>
+    <t>R15, R20</t>
+  </si>
+  <si>
+    <t>20R</t>
+  </si>
+  <si>
+    <t>R5, R19</t>
+  </si>
+  <si>
+    <t>Se crea la posicion 41 con el part Q3 con el valor PMV20XNER
+Se crea la posicion 42 con los parts R15 y R20 con el valor 20R
+Se añade el part R19 a la posicion 26</t>
   </si>
 </sst>
 </file>
@@ -1227,6 +1250,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1239,54 +1263,103 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Bueno" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Encabezado 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Encabezado 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Énfasis1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Énfasis2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Énfasis3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Énfasis4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Énfasis5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Énfasis6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Hipervínculo" xfId="42" builtinId="8"/>
+    <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Salida" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Texto de advertencia" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Texto explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1380,13 +1453,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AD639D9D-BFED-4687-9866-69587ACF8311}" name="Tabla1" displayName="Tabla1" ref="A6:K46" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AD639D9D-BFED-4687-9866-69587ACF8311}" name="Tabla1" displayName="Tabla1" ref="A6:K48" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:K46">
     <sortCondition ref="A6:A46"/>
   </sortState>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{A4EEF5D5-EC32-4E92-A16D-A2C00D09EC58}" name="Position"/>
-    <tableColumn id="10" xr3:uid="{AB092131-4167-465E-A2DF-04757A83F427}" name="NEW" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{AB092131-4167-465E-A2DF-04757A83F427}" name="NEW" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{958FBBFD-8FA4-4642-8441-E180A56F96F0}" name="Qty"/>
     <tableColumn id="3" xr3:uid="{FBAE2CFA-77A4-45AD-9266-0EFC588D4B64}" name="Part"/>
     <tableColumn id="4" xr3:uid="{FB9BFB6E-6495-468E-802B-025835AD898D}" name="Value"/>
@@ -1402,7 +1475,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1698,50 +1771,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K46"/>
+  <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="145.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="145.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:11" ht="16">
+    <row r="2" spans="1:11" ht="15.75">
       <c r="A2" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B2" s="3">
         <f>MAX(_HISTORY!A4:A55)</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="26">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="27">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
       <c r="D3" s="4"/>
     </row>
-    <row r="4" spans="1:11" ht="26">
-      <c r="B4" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="25"/>
+    <row r="4" spans="1:11" ht="27">
+      <c r="B4" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="26"/>
     </row>
     <row r="5" spans="1:11" ht="13.5" customHeight="1">
       <c r="B5" s="6"/>
@@ -1751,16 +1824,16 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>1</v>
@@ -1772,16 +1845,16 @@
         <v>3</v>
       </c>
       <c r="H6" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="I6" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="J6" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="K6" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="J6" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="K6" s="9" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1789,7 +1862,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -1798,13 +1871,13 @@
         <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1812,22 +1885,22 @@
         <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C8">
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1835,22 +1908,22 @@
         <v>3</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C9">
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F9" t="s">
+        <v>68</v>
+      </c>
+      <c r="G9" t="s">
         <v>69</v>
-      </c>
-      <c r="G9" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1858,22 +1931,22 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C10">
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F10" t="s">
+        <v>68</v>
+      </c>
+      <c r="G10" t="s">
         <v>69</v>
-      </c>
-      <c r="G10" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1881,22 +1954,22 @@
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C11">
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1904,32 +1977,32 @@
         <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F12" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G12" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H12" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I12" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J12" s="18"/>
       <c r="K12" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1937,7 +2010,7 @@
         <v>7</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -1946,13 +2019,13 @@
         <v>12</v>
       </c>
       <c r="E13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1960,32 +2033,32 @@
         <v>8</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F14" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G14" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H14" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I14" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J14" s="18"/>
       <c r="K14" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1993,7 +2066,7 @@
         <v>9</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -2002,13 +2075,13 @@
         <v>6</v>
       </c>
       <c r="E15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -2016,26 +2089,26 @@
         <v>10</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G16" t="s">
         <v>14</v>
       </c>
       <c r="J16" s="20"/>
       <c r="K16" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -2043,26 +2116,26 @@
         <v>11</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J17" s="20"/>
       <c r="K17" s="20" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -2070,7 +2143,7 @@
         <v>12</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -2082,14 +2155,14 @@
         <v>10</v>
       </c>
       <c r="F18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J18" s="20"/>
       <c r="K18" s="20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -2097,28 +2170,28 @@
         <v>13</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J19" s="20" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K19" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -2126,19 +2199,19 @@
         <v>14</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E20" t="s">
         <v>13</v>
       </c>
       <c r="F20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G20" t="s">
         <v>14</v>
@@ -2149,7 +2222,7 @@
         <v>15</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -2161,10 +2234,10 @@
         <v>7</v>
       </c>
       <c r="F21" t="s">
+        <v>60</v>
+      </c>
+      <c r="G21" t="s">
         <v>61</v>
-      </c>
-      <c r="G21" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -2172,7 +2245,7 @@
         <v>16</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -2184,10 +2257,10 @@
         <v>18</v>
       </c>
       <c r="F22" t="s">
+        <v>60</v>
+      </c>
+      <c r="G22" t="s">
         <v>61</v>
-      </c>
-      <c r="G22" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -2195,22 +2268,22 @@
         <v>17</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F23" t="s">
+        <v>60</v>
+      </c>
+      <c r="G23" t="s">
         <v>61</v>
-      </c>
-      <c r="G23" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -2218,22 +2291,22 @@
         <v>18</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F24" t="s">
+        <v>60</v>
+      </c>
+      <c r="G24" t="s">
         <v>61</v>
-      </c>
-      <c r="G24" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -2241,22 +2314,22 @@
         <v>19</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F25" t="s">
+        <v>60</v>
+      </c>
+      <c r="G25" t="s">
         <v>61</v>
-      </c>
-      <c r="G25" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -2264,22 +2337,22 @@
         <v>20</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C26">
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F26" t="s">
+        <v>60</v>
+      </c>
+      <c r="G26" t="s">
         <v>61</v>
-      </c>
-      <c r="G26" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -2287,22 +2360,22 @@
         <v>21</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C27">
         <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E27" t="s">
         <v>15</v>
       </c>
       <c r="F27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -2310,22 +2383,22 @@
         <v>22</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C28">
         <v>2</v>
       </c>
       <c r="D28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F28" t="s">
+        <v>60</v>
+      </c>
+      <c r="G28" t="s">
         <v>61</v>
-      </c>
-      <c r="G28" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -2333,22 +2406,22 @@
         <v>23</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C29">
         <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E29" t="s">
         <v>4</v>
       </c>
       <c r="F29" t="s">
+        <v>60</v>
+      </c>
+      <c r="G29" t="s">
         <v>61</v>
-      </c>
-      <c r="G29" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -2356,22 +2429,22 @@
         <v>24</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C30">
         <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E30" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F30" t="s">
+        <v>60</v>
+      </c>
+      <c r="G30" t="s">
         <v>61</v>
-      </c>
-      <c r="G30" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -2379,7 +2452,7 @@
         <v>25</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -2391,10 +2464,10 @@
         <v>16</v>
       </c>
       <c r="F31" t="s">
+        <v>60</v>
+      </c>
+      <c r="G31" t="s">
         <v>61</v>
-      </c>
-      <c r="G31" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -2402,22 +2475,22 @@
         <v>26</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>73</v>
+        <v>134</v>
       </c>
       <c r="C32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D32" t="s">
-        <v>21</v>
+        <v>153</v>
       </c>
       <c r="E32" t="s">
         <v>20</v>
       </c>
       <c r="F32" t="s">
+        <v>60</v>
+      </c>
+      <c r="G32" t="s">
         <v>61</v>
-      </c>
-      <c r="G32" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:11">
@@ -2425,22 +2498,22 @@
         <v>27</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C33">
         <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G33" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="34" spans="1:11">
@@ -2448,22 +2521,22 @@
         <v>28</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C34">
         <v>1</v>
       </c>
       <c r="D34" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E34" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G34" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="35" spans="1:11">
@@ -2471,22 +2544,22 @@
         <v>29</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C35">
         <v>1</v>
       </c>
       <c r="D35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F35" t="s">
+        <v>60</v>
+      </c>
+      <c r="G35" t="s">
         <v>61</v>
-      </c>
-      <c r="G35" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="36" spans="1:11">
@@ -2494,7 +2567,7 @@
         <v>30</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -2503,17 +2576,17 @@
         <v>5</v>
       </c>
       <c r="E36" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G36" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J36" s="20"/>
       <c r="K36" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="37" spans="1:11">
@@ -2521,26 +2594,26 @@
         <v>31</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C37">
         <v>2</v>
       </c>
       <c r="D37" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E37" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F37" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G37" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J37" s="20"/>
       <c r="K37" s="20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="38" spans="1:11">
@@ -2548,26 +2621,26 @@
         <v>32</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C38">
         <v>1</v>
       </c>
       <c r="D38" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E38" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F38" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G38" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J38" s="20"/>
       <c r="K38" s="20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="39" spans="1:11">
@@ -2575,22 +2648,22 @@
         <v>33</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C39">
         <v>1</v>
       </c>
       <c r="D39" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E39" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F39" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G39" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="40" spans="1:11">
@@ -2598,22 +2671,22 @@
         <v>34</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C40">
         <v>1</v>
       </c>
       <c r="D40" t="s">
+        <v>95</v>
+      </c>
+      <c r="E40" t="s">
         <v>96</v>
       </c>
-      <c r="E40" t="s">
-        <v>97</v>
-      </c>
       <c r="F40" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G40" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="41" spans="1:11">
@@ -2621,22 +2694,22 @@
         <v>35</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C41">
         <v>1</v>
       </c>
       <c r="D41" t="s">
+        <v>98</v>
+      </c>
+      <c r="E41" t="s">
         <v>99</v>
       </c>
-      <c r="E41" t="s">
-        <v>100</v>
-      </c>
       <c r="F41" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G41" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="42" spans="1:11">
@@ -2644,22 +2717,22 @@
         <v>36</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C42">
         <v>2</v>
       </c>
       <c r="D42" t="s">
+        <v>101</v>
+      </c>
+      <c r="E42" t="s">
         <v>102</v>
       </c>
-      <c r="E42" t="s">
-        <v>103</v>
-      </c>
       <c r="F42" t="s">
+        <v>60</v>
+      </c>
+      <c r="G42" t="s">
         <v>61</v>
-      </c>
-      <c r="G42" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="43" spans="1:11">
@@ -2667,22 +2740,22 @@
         <v>37</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C43">
         <v>1</v>
       </c>
       <c r="D43" t="s">
+        <v>103</v>
+      </c>
+      <c r="E43" t="s">
         <v>104</v>
       </c>
-      <c r="E43" t="s">
-        <v>105</v>
-      </c>
       <c r="F43" t="s">
+        <v>60</v>
+      </c>
+      <c r="G43" t="s">
         <v>61</v>
-      </c>
-      <c r="G43" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="44" spans="1:11">
@@ -2690,26 +2763,26 @@
         <v>38</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C44">
         <v>1</v>
       </c>
       <c r="D44" t="s">
+        <v>125</v>
+      </c>
+      <c r="E44" t="s">
         <v>126</v>
       </c>
-      <c r="E44" t="s">
+      <c r="F44" t="s">
         <v>127</v>
       </c>
-      <c r="F44" t="s">
+      <c r="G44" t="s">
         <v>128</v>
-      </c>
-      <c r="G44" t="s">
-        <v>129</v>
       </c>
       <c r="J44" s="20"/>
       <c r="K44" s="20" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="45" spans="1:11">
@@ -2717,28 +2790,28 @@
         <v>39</v>
       </c>
       <c r="B45" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45" t="s">
         <v>135</v>
       </c>
-      <c r="C45">
-        <v>1</v>
-      </c>
-      <c r="D45" t="s">
+      <c r="E45" t="s">
+        <v>138</v>
+      </c>
+      <c r="F45" t="s">
+        <v>67</v>
+      </c>
+      <c r="G45" t="s">
+        <v>137</v>
+      </c>
+      <c r="J45" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="K45" s="20" t="s">
         <v>136</v>
-      </c>
-      <c r="E45" t="s">
-        <v>139</v>
-      </c>
-      <c r="F45" t="s">
-        <v>68</v>
-      </c>
-      <c r="G45" t="s">
-        <v>138</v>
-      </c>
-      <c r="J45" s="27" t="s">
-        <v>146</v>
-      </c>
-      <c r="K45" s="20" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="46" spans="1:11">
@@ -2746,36 +2819,82 @@
         <v>40</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C46">
         <v>1</v>
       </c>
       <c r="D46" t="s">
+        <v>139</v>
+      </c>
+      <c r="E46" t="s">
         <v>140</v>
       </c>
-      <c r="E46" t="s">
-        <v>141</v>
-      </c>
       <c r="F46" t="s">
+        <v>60</v>
+      </c>
+      <c r="G46" t="s">
         <v>61</v>
       </c>
-      <c r="G46" t="s">
-        <v>62</v>
+    </row>
+    <row r="47" spans="1:11">
+      <c r="A47">
+        <v>41</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47" t="s">
+        <v>147</v>
+      </c>
+      <c r="E47" t="s">
+        <v>148</v>
+      </c>
+      <c r="F47" t="s">
+        <v>149</v>
+      </c>
+      <c r="G47" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
+      <c r="A48">
+        <v>42</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C48">
+        <v>2</v>
+      </c>
+      <c r="D48" t="s">
+        <v>151</v>
+      </c>
+      <c r="E48" t="s">
+        <v>152</v>
+      </c>
+      <c r="F48" t="s">
+        <v>60</v>
+      </c>
+      <c r="G48" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B4:E4"/>
   </mergeCells>
-  <conditionalFormatting sqref="B7:B46">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="NO">
+  <conditionalFormatting sqref="B7:B48">
+    <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",B7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="YES">
+    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="YES">
       <formula>NOT(ISERROR(SEARCH("YES",B7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",B7)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2801,37 +2920,37 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5396D425-0A04-B64D-B9F7-D3F9797B3C5D}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="51.1640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.85546875" style="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="24">
+    <row r="1" spans="1:4" ht="23.25">
       <c r="A1" s="15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18.75">
+      <c r="A3" s="16" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="20">
-      <c r="A3" s="16" t="s">
+      <c r="B3" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="C3" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="D3" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="D3" s="21" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="16">
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2839,13 +2958,13 @@
         <v>44874</v>
       </c>
       <c r="C4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="D4" s="19" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="64">
+    </row>
+    <row r="5" spans="1:4" ht="60">
       <c r="A5">
         <v>2</v>
       </c>
@@ -2853,13 +2972,13 @@
         <v>44880</v>
       </c>
       <c r="C5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="144">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="135">
       <c r="A6">
         <v>3</v>
       </c>
@@ -2867,13 +2986,13 @@
         <v>44922</v>
       </c>
       <c r="C6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="32">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="30">
       <c r="A7">
         <v>4</v>
       </c>
@@ -2881,13 +3000,13 @@
         <v>44931</v>
       </c>
       <c r="C7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="16">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>5</v>
       </c>
@@ -2895,13 +3014,13 @@
         <v>44958</v>
       </c>
       <c r="C8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="16">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9">
         <v>6</v>
       </c>
@@ -2909,13 +3028,13 @@
         <v>45062</v>
       </c>
       <c r="C9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="64">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="60">
       <c r="A10">
         <v>7</v>
       </c>
@@ -2923,13 +3042,13 @@
         <v>45180</v>
       </c>
       <c r="C10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="16">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11">
         <v>8</v>
       </c>
@@ -2937,13 +3056,13 @@
         <v>45194</v>
       </c>
       <c r="C11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="16">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12">
         <v>9</v>
       </c>
@@ -2951,10 +3070,24 @@
         <v>45195</v>
       </c>
       <c r="C12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>147</v>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="45">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13" s="22">
+        <v>45239</v>
+      </c>
+      <c r="C13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -2973,67 +3106,67 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3" ht="21">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+    </row>
+    <row r="2" spans="1:3" ht="18.75">
+      <c r="A2" s="10" t="s">
         <v>74</v>
-      </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-    </row>
-    <row r="2" spans="1:3" ht="19">
-      <c r="A2" s="10" t="s">
-        <v>75</v>
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="11"/>
     </row>
-    <row r="3" spans="1:3" ht="19">
+    <row r="3" spans="1:3" ht="18.75">
       <c r="A3" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="11"/>
     </row>
-    <row r="4" spans="1:3" ht="19">
+    <row r="4" spans="1:3" ht="18.75">
       <c r="A4" s="10">
         <v>28805</v>
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
     </row>
-    <row r="5" spans="1:3" ht="19">
+    <row r="5" spans="1:3" ht="18.75">
       <c r="A5" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="11"/>
     </row>
-    <row r="6" spans="1:3" ht="19">
+    <row r="6" spans="1:3" ht="18.75">
       <c r="A6" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
     </row>
-    <row r="7" spans="1:3" ht="19">
+    <row r="7" spans="1:3" ht="18.75">
       <c r="A7" s="10"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
     </row>
-    <row r="8" spans="1:3" ht="19">
+    <row r="8" spans="1:3" ht="18.75">
       <c r="A8" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="C8" s="14"/>
+    </row>
+    <row r="9" spans="1:3" ht="18.75">
+      <c r="A9" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="C8" s="14"/>
-    </row>
-    <row r="9" spans="1:3" ht="19">
-      <c r="A9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>81</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>82</v>
       </c>
       <c r="C9" s="11"/>
     </row>

</xml_diff>

<commit_message>
Add C11 y R22.
</commit_message>
<xml_diff>
--- a/02.HARDWARE/V2-ROVER R-1/02.BOM/BATT_DCDC.xlsx
+++ b/02.HARDWARE/V2-ROVER R-1/02.BOM/BATT_DCDC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Team Dropbox\JRODRIGUEZ\Repositorios\01.Rover\02.HARDWARE\V2-ROVER R-1\02.BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37FC938C-0E93-41CD-8B1D-3D5DE38DAD55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D9637D-5AC1-4BDA-8F62-583809AC8421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BATT_DCDC" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="157">
   <si>
     <t>Document property of:</t>
   </si>
@@ -221,9 +221,6 @@
     <t>47uF 25V</t>
   </si>
   <si>
-    <t>C2, C5, C6,C8 C24</t>
-  </si>
-  <si>
     <t>100nF, 25V, X7R o X5R</t>
   </si>
   <si>
@@ -452,9 +449,6 @@
     <t>N.A</t>
   </si>
   <si>
-    <t>R7,R21</t>
-  </si>
-  <si>
     <t>4k3</t>
   </si>
   <si>
@@ -522,6 +516,16 @@
   </si>
   <si>
     <t>20R</t>
+  </si>
+  <si>
+    <t>R7,R21,R22</t>
+  </si>
+  <si>
+    <t>C2, C5, C6,C8 C24,C11</t>
+  </si>
+  <si>
+    <t>Se añade a la posicion 35 el part R22 se cambia la cantidad de 2 a 3
+Se añade a la posicion 5 el part C11 se cambia la cantidad de 5 a 6</t>
   </si>
 </sst>
 </file>
@@ -871,9 +875,6 @@
     <xf numFmtId="14" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -957,12 +958,19 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -980,7 +988,7 @@
   <autoFilter ref="A6:L48" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Position"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="NEW"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="NEW" dataDxfId="0"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Assembly"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Qty"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Part"/>
@@ -1286,16 +1294,16 @@
   </sheetPr>
   <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" style="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" style="42" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" style="43" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" style="22" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="41" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" style="42" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" style="21" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="30.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="20.85546875" bestFit="1" customWidth="1"/>
@@ -1306,82 +1314,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18.75" customHeight="1">
-      <c r="B1" s="23"/>
-      <c r="C1" s="24"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="23"/>
     </row>
     <row r="2" spans="1:12" ht="20.25" customHeight="1">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="26">
+      <c r="B2" s="25">
         <f>MAX(_HISTORY!A4:A55)</f>
-        <v>12</v>
-      </c>
-      <c r="C2" s="27"/>
+        <v>13</v>
+      </c>
+      <c r="C2" s="26"/>
     </row>
     <row r="3" spans="1:12" ht="29.25" customHeight="1">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="28">
-        <f>VLOOKUP(B2,_HISTORY!A3:D15,2)</f>
-        <v>45545</v>
-      </c>
-      <c r="C3" s="28"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="30"/>
+      <c r="B3" s="27">
+        <f>VLOOKUP(B2,_HISTORY!A3:D100,2)</f>
+        <v>45553</v>
+      </c>
+      <c r="C3" s="27"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="29"/>
     </row>
     <row r="4" spans="1:12" ht="30" customHeight="1">
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="45"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="47"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="46"/>
     </row>
     <row r="5" spans="1:12" ht="30.75" customHeight="1">
-      <c r="B5" s="31"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="34"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="33"/>
     </row>
     <row r="6" spans="1:12" ht="18.75" customHeight="1">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="37" t="s">
+      <c r="C6" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="35" t="s">
+      <c r="D6" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="37" t="s">
+      <c r="E6" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="37" t="s">
+      <c r="F6" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="G6" s="37" t="s">
+      <c r="G6" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="H6" s="37" t="s">
+      <c r="H6" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="I6" s="37" t="s">
+      <c r="I6" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="J6" s="37" t="s">
+      <c r="J6" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="K6" s="37" t="s">
+      <c r="K6" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="L6" s="37" t="s">
+      <c r="L6" s="36" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1389,10 +1397,10 @@
       <c r="A7" s="17">
         <v>1</v>
       </c>
-      <c r="B7" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" s="24"/>
+      <c r="B7" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="23"/>
       <c r="D7" s="17">
         <v>2</v>
       </c>
@@ -1413,10 +1421,10 @@
       <c r="A8" s="17">
         <v>2</v>
       </c>
-      <c r="B8" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" s="24"/>
+      <c r="B8" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="23"/>
       <c r="D8" s="17">
         <v>2</v>
       </c>
@@ -1437,10 +1445,10 @@
       <c r="A9" s="17">
         <v>3</v>
       </c>
-      <c r="B9" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" s="24"/>
+      <c r="B9" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="23"/>
       <c r="D9" s="17">
         <v>2</v>
       </c>
@@ -1461,10 +1469,10 @@
       <c r="A10" s="17">
         <v>4</v>
       </c>
-      <c r="B10" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C10" s="24"/>
+      <c r="B10" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="23"/>
       <c r="D10" s="17">
         <v>2</v>
       </c>
@@ -1485,18 +1493,18 @@
       <c r="A11" s="17">
         <v>5</v>
       </c>
-      <c r="B11" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" s="24"/>
+      <c r="B11" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="C11" s="23"/>
       <c r="D11" s="17">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E11" t="s">
+        <v>155</v>
+      </c>
+      <c r="F11" t="s">
         <v>55</v>
-      </c>
-      <c r="F11" t="s">
-        <v>56</v>
       </c>
       <c r="G11" t="s">
         <v>45</v>
@@ -1506,55 +1514,55 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="18.75" customHeight="1">
-      <c r="A12" s="38">
+      <c r="A12" s="37">
         <v>6</v>
       </c>
-      <c r="B12" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" s="39"/>
-      <c r="D12" s="40" t="s">
-        <v>57</v>
-      </c>
-      <c r="E12" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="F12" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="G12" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="H12" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="I12" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="J12" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="K12" s="39"/>
-      <c r="L12" s="39" t="s">
-        <v>57</v>
+      <c r="B12" s="49" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="38"/>
+      <c r="D12" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="G12" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="H12" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="I12" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="J12" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="K12" s="38"/>
+      <c r="L12" s="38" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="18.75" customHeight="1">
       <c r="A13" s="17">
         <v>7</v>
       </c>
-      <c r="B13" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" s="24"/>
+      <c r="B13" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="23"/>
       <c r="D13" s="17">
         <v>1</v>
       </c>
       <c r="E13" t="s">
+        <v>57</v>
+      </c>
+      <c r="F13" t="s">
         <v>58</v>
-      </c>
-      <c r="F13" t="s">
-        <v>59</v>
       </c>
       <c r="G13" t="s">
         <v>45</v>
@@ -1564,278 +1572,278 @@
       </c>
     </row>
     <row r="14" spans="1:12" ht="18.75" customHeight="1">
-      <c r="A14" s="38">
+      <c r="A14" s="37">
         <v>8</v>
       </c>
-      <c r="B14" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" s="39"/>
-      <c r="D14" s="40" t="s">
-        <v>57</v>
-      </c>
-      <c r="E14" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="F14" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="G14" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="H14" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="I14" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="J14" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="K14" s="39"/>
-      <c r="L14" s="39" t="s">
-        <v>57</v>
+      <c r="B14" s="49" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="38"/>
+      <c r="D14" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="G14" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="H14" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="I14" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="J14" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="K14" s="38"/>
+      <c r="L14" s="38" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="18.75" customHeight="1">
       <c r="A15" s="17">
         <v>9</v>
       </c>
-      <c r="B15" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" s="24"/>
+      <c r="B15" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="23"/>
       <c r="D15" s="17">
         <v>1</v>
       </c>
       <c r="E15" t="s">
+        <v>59</v>
+      </c>
+      <c r="F15" t="s">
         <v>60</v>
-      </c>
-      <c r="F15" t="s">
-        <v>61</v>
       </c>
       <c r="G15" t="s">
         <v>45</v>
       </c>
       <c r="H15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="19.5" customHeight="1">
       <c r="A16" s="17">
         <v>10</v>
       </c>
-      <c r="B16" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" s="24"/>
+      <c r="B16" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="23"/>
       <c r="D16" s="17">
         <v>1</v>
       </c>
       <c r="E16" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" t="s">
         <v>63</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>64</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>65</v>
-      </c>
-      <c r="H16" t="s">
-        <v>66</v>
       </c>
       <c r="K16" s="5"/>
       <c r="L16" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="19.5" customHeight="1">
       <c r="A17" s="17">
         <v>11</v>
       </c>
-      <c r="B17" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" s="24"/>
+      <c r="B17" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="23"/>
       <c r="D17" s="17">
         <v>1</v>
       </c>
       <c r="E17" t="s">
+        <v>67</v>
+      </c>
+      <c r="F17" t="s">
         <v>68</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H17" t="s">
         <v>69</v>
-      </c>
-      <c r="G17" t="s">
-        <v>65</v>
-      </c>
-      <c r="H17" t="s">
-        <v>70</v>
       </c>
       <c r="K17" s="5"/>
       <c r="L17" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="19.5" customHeight="1">
       <c r="A18" s="17">
         <v>12</v>
       </c>
-      <c r="B18" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" s="24"/>
+      <c r="B18" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="23"/>
       <c r="D18" s="17">
         <v>1</v>
       </c>
       <c r="E18" t="s">
+        <v>71</v>
+      </c>
+      <c r="F18" t="s">
         <v>72</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>73</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>74</v>
-      </c>
-      <c r="H18" t="s">
-        <v>75</v>
       </c>
       <c r="K18" s="5"/>
       <c r="L18" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="19.5" customHeight="1">
       <c r="A19" s="17">
         <v>13</v>
       </c>
-      <c r="B19" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" s="24"/>
+      <c r="B19" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="23"/>
       <c r="D19" s="17">
         <v>1</v>
       </c>
       <c r="E19" t="s">
+        <v>76</v>
+      </c>
+      <c r="F19" t="s">
         <v>77</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>78</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>79</v>
       </c>
-      <c r="H19" t="s">
+      <c r="K19" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="K19" s="5" t="s">
+      <c r="L19" s="5" t="s">
         <v>81</v>
-      </c>
-      <c r="L19" s="5" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="18.75" customHeight="1">
       <c r="A20" s="17">
         <v>14</v>
       </c>
-      <c r="B20" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" s="24"/>
+      <c r="B20" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="23"/>
       <c r="D20" s="17">
         <v>1</v>
       </c>
       <c r="E20" t="s">
+        <v>82</v>
+      </c>
+      <c r="F20" t="s">
         <v>83</v>
       </c>
-      <c r="F20" t="s">
-        <v>84</v>
-      </c>
       <c r="G20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="18.75" customHeight="1">
       <c r="A21" s="17">
         <v>15</v>
       </c>
-      <c r="B21" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" s="24"/>
+      <c r="B21" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="23"/>
       <c r="D21" s="17">
         <v>1</v>
       </c>
       <c r="E21" t="s">
+        <v>84</v>
+      </c>
+      <c r="F21" t="s">
         <v>85</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>86</v>
-      </c>
-      <c r="G21" t="s">
-        <v>87</v>
       </c>
       <c r="H21" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="18.75" customHeight="1">
-      <c r="A22" s="38">
+      <c r="A22" s="37">
         <v>16</v>
       </c>
-      <c r="B22" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="C22" s="39"/>
-      <c r="D22" s="40" t="s">
-        <v>57</v>
-      </c>
-      <c r="E22" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="F22" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="G22" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="H22" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="I22" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="J22" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="K22" s="39"/>
-      <c r="L22" s="39" t="s">
-        <v>57</v>
+      <c r="B22" s="49" t="s">
+        <v>87</v>
+      </c>
+      <c r="C22" s="38"/>
+      <c r="D22" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="F22" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="G22" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="H22" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="I22" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="J22" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="K22" s="38"/>
+      <c r="L22" s="38" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="18.75" customHeight="1">
       <c r="A23" s="17">
         <v>17</v>
       </c>
-      <c r="B23" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C23" s="24"/>
+      <c r="B23" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="23"/>
       <c r="D23" s="17">
         <v>1</v>
       </c>
       <c r="E23" t="s">
+        <v>88</v>
+      </c>
+      <c r="F23" t="s">
         <v>89</v>
       </c>
-      <c r="F23" t="s">
-        <v>90</v>
-      </c>
       <c r="G23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H23" t="s">
         <v>46</v>
@@ -1845,21 +1853,21 @@
       <c r="A24" s="17">
         <v>18</v>
       </c>
-      <c r="B24" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C24" s="24"/>
+      <c r="B24" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" s="23"/>
       <c r="D24" s="17">
         <v>1</v>
       </c>
       <c r="E24" t="s">
+        <v>90</v>
+      </c>
+      <c r="F24" t="s">
         <v>91</v>
       </c>
-      <c r="F24" t="s">
-        <v>92</v>
-      </c>
       <c r="G24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H24" t="s">
         <v>46</v>
@@ -1869,21 +1877,21 @@
       <c r="A25" s="17">
         <v>19</v>
       </c>
-      <c r="B25" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C25" s="24"/>
+      <c r="B25" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="23"/>
       <c r="D25" s="17">
         <v>1</v>
       </c>
       <c r="E25" t="s">
+        <v>92</v>
+      </c>
+      <c r="F25" t="s">
         <v>93</v>
       </c>
-      <c r="F25" t="s">
-        <v>94</v>
-      </c>
       <c r="G25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H25" t="s">
         <v>46</v>
@@ -1893,21 +1901,21 @@
       <c r="A26" s="17">
         <v>20</v>
       </c>
-      <c r="B26" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C26" s="24"/>
+      <c r="B26" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="23"/>
       <c r="D26" s="17">
         <v>1</v>
       </c>
       <c r="E26" t="s">
+        <v>94</v>
+      </c>
+      <c r="F26" t="s">
         <v>95</v>
       </c>
-      <c r="F26" t="s">
-        <v>96</v>
-      </c>
       <c r="G26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H26" t="s">
         <v>46</v>
@@ -1917,21 +1925,21 @@
       <c r="A27" s="17">
         <v>21</v>
       </c>
-      <c r="B27" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C27" s="24"/>
+      <c r="B27" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" s="23"/>
       <c r="D27" s="17">
         <v>1</v>
       </c>
       <c r="E27" t="s">
+        <v>96</v>
+      </c>
+      <c r="F27" t="s">
         <v>97</v>
       </c>
-      <c r="F27" t="s">
-        <v>98</v>
-      </c>
       <c r="G27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H27" t="s">
         <v>49</v>
@@ -1941,21 +1949,21 @@
       <c r="A28" s="17">
         <v>22</v>
       </c>
-      <c r="B28" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C28" s="24"/>
+      <c r="B28" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28" s="23"/>
       <c r="D28" s="17">
         <v>2</v>
       </c>
       <c r="E28" t="s">
+        <v>98</v>
+      </c>
+      <c r="F28" t="s">
         <v>99</v>
       </c>
-      <c r="F28" t="s">
-        <v>100</v>
-      </c>
       <c r="G28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H28" t="s">
         <v>46</v>
@@ -1965,21 +1973,21 @@
       <c r="A29" s="17">
         <v>23</v>
       </c>
-      <c r="B29" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C29" s="24"/>
+      <c r="B29" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" s="23"/>
       <c r="D29" s="17">
         <v>1</v>
       </c>
       <c r="E29" t="s">
+        <v>100</v>
+      </c>
+      <c r="F29" t="s">
         <v>101</v>
       </c>
-      <c r="F29" t="s">
-        <v>102</v>
-      </c>
       <c r="G29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H29" t="s">
         <v>46</v>
@@ -1989,21 +1997,21 @@
       <c r="A30" s="17">
         <v>24</v>
       </c>
-      <c r="B30" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C30" s="24"/>
+      <c r="B30" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" s="23"/>
       <c r="D30" s="17">
         <v>1</v>
       </c>
       <c r="E30" t="s">
+        <v>102</v>
+      </c>
+      <c r="F30" t="s">
         <v>103</v>
       </c>
-      <c r="F30" t="s">
-        <v>104</v>
-      </c>
       <c r="G30" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H30" t="s">
         <v>46</v>
@@ -2013,21 +2021,21 @@
       <c r="A31" s="17">
         <v>25</v>
       </c>
-      <c r="B31" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C31" s="24"/>
+      <c r="B31" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" s="23"/>
       <c r="D31" s="17">
         <v>1</v>
       </c>
       <c r="E31" t="s">
+        <v>104</v>
+      </c>
+      <c r="F31" t="s">
         <v>105</v>
       </c>
-      <c r="F31" t="s">
-        <v>106</v>
-      </c>
       <c r="G31" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H31" t="s">
         <v>46</v>
@@ -2037,21 +2045,21 @@
       <c r="A32" s="17">
         <v>26</v>
       </c>
-      <c r="B32" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C32" s="24"/>
+      <c r="B32" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C32" s="23"/>
       <c r="D32" s="17">
         <v>2</v>
       </c>
       <c r="E32" t="s">
+        <v>106</v>
+      </c>
+      <c r="F32" t="s">
         <v>107</v>
       </c>
-      <c r="F32" t="s">
-        <v>108</v>
-      </c>
       <c r="G32" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H32" t="s">
         <v>46</v>
@@ -2061,21 +2069,21 @@
       <c r="A33" s="17">
         <v>27</v>
       </c>
-      <c r="B33" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C33" s="24"/>
+      <c r="B33" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" s="23"/>
       <c r="D33" s="17">
         <v>1</v>
       </c>
       <c r="E33" t="s">
+        <v>108</v>
+      </c>
+      <c r="F33" t="s">
         <v>109</v>
       </c>
-      <c r="F33" t="s">
-        <v>110</v>
-      </c>
       <c r="G33" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H33" t="s">
         <v>49</v>
@@ -2085,21 +2093,21 @@
       <c r="A34" s="17">
         <v>28</v>
       </c>
-      <c r="B34" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C34" s="24"/>
+      <c r="B34" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C34" s="23"/>
       <c r="D34" s="17">
         <v>1</v>
       </c>
       <c r="E34" t="s">
+        <v>110</v>
+      </c>
+      <c r="F34" t="s">
         <v>111</v>
       </c>
-      <c r="F34" t="s">
-        <v>112</v>
-      </c>
       <c r="G34" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H34" t="s">
         <v>49</v>
@@ -2109,21 +2117,21 @@
       <c r="A35" s="17">
         <v>29</v>
       </c>
-      <c r="B35" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C35" s="24"/>
+      <c r="B35" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C35" s="23"/>
       <c r="D35" s="17">
         <v>1</v>
       </c>
       <c r="E35" t="s">
+        <v>112</v>
+      </c>
+      <c r="F35" t="s">
         <v>113</v>
       </c>
-      <c r="F35" t="s">
-        <v>114</v>
-      </c>
       <c r="G35" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H35" t="s">
         <v>46</v>
@@ -2133,102 +2141,102 @@
       <c r="A36" s="17">
         <v>30</v>
       </c>
-      <c r="B36" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C36" s="24"/>
+      <c r="B36" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36" s="23"/>
       <c r="D36" s="17">
         <v>1</v>
       </c>
       <c r="E36" t="s">
+        <v>114</v>
+      </c>
+      <c r="F36" t="s">
         <v>115</v>
       </c>
-      <c r="F36" t="s">
+      <c r="G36" t="s">
+        <v>86</v>
+      </c>
+      <c r="H36" t="s">
         <v>116</v>
-      </c>
-      <c r="G36" t="s">
-        <v>87</v>
-      </c>
-      <c r="H36" t="s">
-        <v>117</v>
       </c>
       <c r="K36" s="5"/>
       <c r="L36" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="18.75" customHeight="1">
       <c r="A37" s="17">
         <v>31</v>
       </c>
-      <c r="B37" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C37" s="24"/>
+      <c r="B37" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C37" s="23"/>
       <c r="D37" s="17">
         <v>2</v>
       </c>
       <c r="E37" t="s">
+        <v>118</v>
+      </c>
+      <c r="F37" t="s">
         <v>119</v>
       </c>
-      <c r="F37" t="s">
+      <c r="G37" t="s">
         <v>120</v>
       </c>
-      <c r="G37" t="s">
+      <c r="H37" t="s">
         <v>121</v>
-      </c>
-      <c r="H37" t="s">
-        <v>122</v>
       </c>
       <c r="K37" s="5"/>
       <c r="L37" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="18.75" customHeight="1">
       <c r="A38" s="17">
         <v>32</v>
       </c>
-      <c r="B38" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C38" s="24"/>
+      <c r="B38" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C38" s="23"/>
       <c r="D38" s="17">
         <v>1</v>
       </c>
       <c r="E38" t="s">
+        <v>123</v>
+      </c>
+      <c r="F38" t="s">
         <v>124</v>
       </c>
-      <c r="F38" t="s">
+      <c r="G38" t="s">
+        <v>120</v>
+      </c>
+      <c r="H38" t="s">
         <v>125</v>
-      </c>
-      <c r="G38" t="s">
-        <v>121</v>
-      </c>
-      <c r="H38" t="s">
-        <v>126</v>
       </c>
       <c r="K38" s="5"/>
       <c r="L38" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="18.75" customHeight="1">
       <c r="A39" s="17">
         <v>33</v>
       </c>
-      <c r="B39" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C39" s="24"/>
+      <c r="B39" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C39" s="23"/>
       <c r="D39" s="17">
         <v>1</v>
       </c>
       <c r="E39" t="s">
+        <v>127</v>
+      </c>
+      <c r="F39" t="s">
         <v>128</v>
-      </c>
-      <c r="F39" t="s">
-        <v>129</v>
       </c>
       <c r="G39" t="s">
         <v>45</v>
@@ -2241,18 +2249,18 @@
       <c r="A40" s="17">
         <v>34</v>
       </c>
-      <c r="B40" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C40" s="24"/>
+      <c r="B40" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C40" s="23"/>
       <c r="D40" s="17">
         <v>1</v>
       </c>
       <c r="E40" t="s">
+        <v>129</v>
+      </c>
+      <c r="F40" t="s">
         <v>130</v>
-      </c>
-      <c r="F40" t="s">
-        <v>131</v>
       </c>
       <c r="G40" t="s">
         <v>45</v>
@@ -2265,21 +2273,21 @@
       <c r="A41" s="17">
         <v>35</v>
       </c>
-      <c r="B41" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="C41" s="24"/>
+      <c r="B41" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="C41" s="23"/>
       <c r="D41" s="17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E41" t="s">
-        <v>132</v>
+        <v>154</v>
       </c>
       <c r="F41" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G41" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H41" t="s">
         <v>49</v>
@@ -2289,21 +2297,21 @@
       <c r="A42" s="17">
         <v>36</v>
       </c>
-      <c r="B42" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="C42" s="24"/>
+      <c r="B42" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="C42" s="23"/>
       <c r="D42" s="17">
         <v>3</v>
       </c>
       <c r="E42" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F42" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G42" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H42" t="s">
         <v>46</v>
@@ -2313,21 +2321,21 @@
       <c r="A43" s="17">
         <v>37</v>
       </c>
-      <c r="B43" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C43" s="24"/>
+      <c r="B43" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C43" s="23"/>
       <c r="D43" s="17">
         <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F43" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G43" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H43" t="s">
         <v>46</v>
@@ -2337,77 +2345,77 @@
       <c r="A44" s="17">
         <v>38</v>
       </c>
-      <c r="B44" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C44" s="24"/>
+      <c r="B44" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C44" s="23"/>
       <c r="D44" s="17">
         <v>1</v>
       </c>
       <c r="E44" t="s">
+        <v>136</v>
+      </c>
+      <c r="F44" t="s">
+        <v>137</v>
+      </c>
+      <c r="G44" t="s">
         <v>138</v>
       </c>
-      <c r="F44" t="s">
+      <c r="H44" t="s">
         <v>139</v>
-      </c>
-      <c r="G44" t="s">
-        <v>140</v>
-      </c>
-      <c r="H44" t="s">
-        <v>141</v>
       </c>
       <c r="K44" s="5"/>
       <c r="L44" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="45" spans="1:12" ht="18.75" customHeight="1">
       <c r="A45" s="17">
         <v>39</v>
       </c>
-      <c r="B45" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="C45" s="24"/>
+      <c r="B45" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="C45" s="23"/>
       <c r="D45" s="17">
         <v>1</v>
       </c>
       <c r="E45" t="s">
+        <v>141</v>
+      </c>
+      <c r="F45" t="s">
+        <v>142</v>
+      </c>
+      <c r="G45" t="s">
+        <v>120</v>
+      </c>
+      <c r="H45" t="s">
         <v>143</v>
       </c>
-      <c r="F45" t="s">
+      <c r="K45" s="40"/>
+      <c r="L45" s="5" t="s">
         <v>144</v>
-      </c>
-      <c r="G45" t="s">
-        <v>121</v>
-      </c>
-      <c r="H45" t="s">
-        <v>145</v>
-      </c>
-      <c r="K45" s="41"/>
-      <c r="L45" s="5" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="46" spans="1:12" ht="18.75" customHeight="1">
       <c r="A46" s="17">
         <v>40</v>
       </c>
-      <c r="B46" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C46" s="24"/>
+      <c r="B46" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C46" s="23"/>
       <c r="D46" s="17">
         <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F46" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G46" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H46" t="s">
         <v>46</v>
@@ -2417,55 +2425,55 @@
       <c r="A47" s="17">
         <v>41</v>
       </c>
-      <c r="B47" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="C47" s="24" t="s">
+      <c r="B47" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="C47" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="D47" s="17">
+        <v>1</v>
+      </c>
+      <c r="E47" t="s">
+        <v>148</v>
+      </c>
+      <c r="F47" t="s">
         <v>149</v>
       </c>
-      <c r="D47" s="17">
-        <v>1</v>
-      </c>
-      <c r="E47" t="s">
+      <c r="G47" t="s">
+        <v>149</v>
+      </c>
+      <c r="H47" t="s">
         <v>150</v>
       </c>
-      <c r="F47" t="s">
+      <c r="L47" s="5" t="s">
         <v>151</v>
-      </c>
-      <c r="G47" t="s">
-        <v>151</v>
-      </c>
-      <c r="H47" t="s">
-        <v>152</v>
-      </c>
-      <c r="L47" s="5" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="48" spans="1:12" ht="18.75" customHeight="1">
       <c r="A48" s="17">
         <v>42</v>
       </c>
-      <c r="B48" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C48" s="24" t="s">
-        <v>149</v>
+      <c r="B48" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C48" s="23" t="s">
+        <v>147</v>
       </c>
       <c r="D48" s="17">
         <v>2</v>
       </c>
       <c r="E48" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F48" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G48" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H48" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -2486,8 +2494,8 @@
   </sheetPr>
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2560,7 +2568,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30">
+    <row r="7" spans="1:4">
       <c r="A7" s="17">
         <v>4</v>
       </c>
@@ -2686,8 +2694,19 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="18.75" customHeight="1">
-      <c r="B16" s="21"/>
+    <row r="16" spans="1:4" ht="30">
+      <c r="A16" s="12">
+        <v>13</v>
+      </c>
+      <c r="B16" s="27">
+        <v>45553</v>
+      </c>
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>156</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2710,11 +2729,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" customHeight="1">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
     </row>
     <row r="2" spans="1:3" ht="18.75" customHeight="1">
       <c r="A2" s="1" t="s">

</xml_diff>